<commit_message>
commit changes to raw data and description
of the data
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63295E13-3860-4F48-9C16-3ACEC75465A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566560C3-3909-458B-8238-E2A0204B409B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3555" yWindow="3098" windowWidth="14400" windowHeight="8182" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>Height</t>
   </si>
@@ -74,22 +74,37 @@
     <t>identified gender (male/female/other)</t>
   </si>
   <si>
+    <t>waist-size</t>
+  </si>
+  <si>
+    <t>size of the waist in inches</t>
+  </si>
+  <si>
     <t>eye-color</t>
   </si>
   <si>
+    <t>color of the individuals eye</t>
+  </si>
+  <si>
+    <t>character variable</t>
+  </si>
+  <si>
+    <t>Waist-size</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
     <t>black</t>
   </si>
   <si>
     <t>green</t>
   </si>
   <si>
-    <t>blue</t>
-  </si>
-  <si>
     <t>brown</t>
   </si>
   <si>
-    <t>waist-size</t>
+    <t>Eye-color</t>
   </si>
 </sst>
 </file>
@@ -419,7 +434,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -435,10 +450,10 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
@@ -451,11 +466,11 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2">
+      <c r="D2">
         <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
@@ -468,11 +483,11 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3">
-        <v>32</v>
+      <c r="D3">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
@@ -485,11 +500,11 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4">
-        <v>31</v>
+      <c r="D4">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
@@ -502,11 +517,11 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5">
-        <v>25</v>
+      <c r="D5">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
@@ -519,11 +534,11 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6">
-        <v>26</v>
+      <c r="D6">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
@@ -536,11 +551,11 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7">
-        <v>28</v>
+      <c r="D7">
+        <v>55</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
@@ -553,11 +568,11 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8">
-        <v>34</v>
+      <c r="D8">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
@@ -570,11 +585,11 @@
       <c r="C9" t="s">
         <v>3</v>
       </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9">
-        <v>32</v>
+      <c r="D9">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
@@ -587,11 +602,11 @@
       <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10">
-        <v>45</v>
+      <c r="D10">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
@@ -604,11 +619,11 @@
       <c r="C11" t="s">
         <v>3</v>
       </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11">
-        <v>67</v>
+      <c r="D11">
+        <v>55</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
@@ -618,11 +633,11 @@
       <c r="C12" t="s">
         <v>4</v>
       </c>
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12">
-        <v>45</v>
+      <c r="D12">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
@@ -635,11 +650,11 @@
       <c r="C13" t="s">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13">
-        <v>30</v>
+      <c r="D13">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
@@ -652,11 +667,11 @@
       <c r="C14" t="s">
         <v>3</v>
       </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14">
-        <v>26</v>
+      <c r="D14">
+        <v>30</v>
+      </c>
+      <c r="E14" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
@@ -669,24 +684,25 @@
       <c r="C15" t="s">
         <v>3</v>
       </c>
-      <c r="D15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15">
-        <v>25</v>
+      <c r="D15">
+        <v>24</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A2C8F0-62B4-4D60-B490-D490A3E0B40F}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -740,6 +756,28 @@
         <v>14</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>